<commit_message>
Add schedule entries for registration and closing; update room display names
</commit_message>
<xml_diff>
--- a/public/devfest-armenia-2025 schedulelist.xlsx
+++ b/public/devfest-armenia-2025 schedulelist.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>Day</t>
   </si>
@@ -32,12 +32,18 @@
     <t>Sat</t>
   </si>
   <si>
+    <t>10:00am - 10:20am</t>
+  </si>
+  <si>
+    <t>Hall A</t>
+  </si>
+  <si>
+    <t>Registration Start</t>
+  </si>
+  <si>
     <t>10:20am - 10:40am</t>
   </si>
   <si>
-    <t>Hall A</t>
-  </si>
-  <si>
     <t>Opening</t>
   </si>
   <si>
@@ -50,7 +56,7 @@
     <t>Seda Sahakyan</t>
   </si>
   <si>
-    <t>Hall B (Wokshops)</t>
+    <t>Hall B</t>
   </si>
   <si>
     <t>WebAI in Action: AI-Powered Accessibility Testing in Chrome</t>
@@ -240,6 +246,12 @@
   </si>
   <si>
     <t>Carlos Sanchez</t>
+  </si>
+  <si>
+    <t>06:10pm - 06:30pm</t>
+  </si>
+  <si>
+    <t>Closing</t>
   </si>
 </sst>
 </file>
@@ -296,7 +308,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -346,25 +358,22 @@
       <c r="D3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="0" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5">
@@ -372,16 +381,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -389,16 +398,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="7">
@@ -406,16 +415,16 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="E7" s="0" t="s">
         <v>22</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="8">
@@ -423,16 +432,16 @@
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="E8" s="0" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -440,12 +449,15 @@
         <v>5</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="E9" s="0" t="s">
         <v>28</v>
       </c>
     </row>
@@ -457,27 +469,27 @@
         <v>29</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>28</v>
+      <c r="E11" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12">
@@ -485,16 +497,13 @@
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
@@ -502,16 +511,16 @@
         <v>5</v>
       </c>
       <c r="B13" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14">
@@ -519,16 +528,16 @@
         <v>5</v>
       </c>
       <c r="B14" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="E14" s="0" t="s">
         <v>40</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15">
@@ -536,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="E15" s="0" t="s">
         <v>43</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="16">
@@ -553,16 +562,16 @@
         <v>5</v>
       </c>
       <c r="B16" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" s="0" t="s">
+      <c r="E16" s="0" t="s">
         <v>46</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17">
@@ -570,16 +579,16 @@
         <v>5</v>
       </c>
       <c r="B17" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="E17" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18">
@@ -587,16 +596,16 @@
         <v>5</v>
       </c>
       <c r="B18" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="E18" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19">
@@ -604,13 +613,16 @@
         <v>5</v>
       </c>
       <c r="B19" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>28</v>
+      <c r="E19" s="0" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20">
@@ -618,16 +630,13 @@
         <v>5</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21">
@@ -635,16 +644,16 @@
         <v>5</v>
       </c>
       <c r="B21" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" s="0" t="s">
+      <c r="E21" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22">
@@ -652,16 +661,16 @@
         <v>5</v>
       </c>
       <c r="B22" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="0" t="s">
+      <c r="E22" s="0" t="s">
         <v>62</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23">
@@ -669,16 +678,16 @@
         <v>5</v>
       </c>
       <c r="B23" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D23" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="E23" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="24">
@@ -686,16 +695,16 @@
         <v>5</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="E24" s="0" t="s">
         <v>68</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25">
@@ -703,16 +712,16 @@
         <v>5</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D25" s="0" t="s">
+      <c r="E25" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26">
@@ -720,16 +729,47 @@
         <v>5</v>
       </c>
       <c r="B26" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="0" t="s">
+      <c r="E26" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="0" t="s">
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>75</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>